<commit_message>
CHG: finish user can't choose same course_id and cant't choose not there dept course
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruserxd/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruserxd/Desktop/college/2down/DB_CourseSelectionSystem/Menu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC008919-DCFC-624E-990B-B25543BB7358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88827BF-B88D-054D-B167-9736E83D7DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="740" windowWidth="28260" windowHeight="17200" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
@@ -685,7 +685,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -721,7 +721,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:3">

</xml_diff>

<commit_message>
CHG:finish course_time_conflict AND is_course_of_capacity then it will give a error message
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruserxd/Desktop/college/2down/DB_CourseSelectionSystem/Menu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A88827BF-B88D-054D-B167-9736E83D7DC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1471932-AC60-AF41-A4DB-6B2092BAACED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="740" windowWidth="28260" windowHeight="17200" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
@@ -684,8 +684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD11E25E-09B4-E24C-BF54-4E794C068EA7}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -729,7 +729,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -737,7 +737,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:3">

</xml_diff>

<commit_message>
CHG: 1. If user successfully choose course and the curNumOfSelect of the course will be updated      2. Check user Selcted not have the same course_name ADD: for Course table add some same name course
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruserxd/Desktop/college/2down/DB_CourseSelectionSystem/Menu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1471932-AC60-AF41-A4DB-6B2092BAACED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6282BC-A45B-DF4E-95A7-2863BF1CB98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="740" windowWidth="28260" windowHeight="17200" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
+    <workbookView xWindow="560" yWindow="740" windowWidth="28260" windowHeight="18380" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
   <sheets>
     <sheet name="功能表" sheetId="1" r:id="rId1"/>
@@ -685,7 +685,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -745,7 +745,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16">

</xml_diff>

<commit_message>
CHG: finish check is_credit_Over_limit
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruserxd/Desktop/college/2down/DB_CourseSelectionSystem/Menu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6282BC-A45B-DF4E-95A7-2863BF1CB98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{170140E7-BE43-FF43-84AA-8F461E19E618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="560" yWindow="740" windowWidth="28260" windowHeight="18380" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
@@ -753,7 +753,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:3">

</xml_diff>

<commit_message>
add alert when user withdraw required course
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d9e3a679e5b315e6/桌面/DB/DB_CourseSelectionSystem/Menu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack9\Desktop\DB\DB_CourseSelectionSystem\Menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{170140E7-BE43-FF43-84AA-8F461E19E618}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73788B3B-B970-45D4-B262-18B695882BDD}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD8855B-D54F-4B17-9581-988D747E6C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
   <sheets>
     <sheet name="功能表" sheetId="1" r:id="rId1"/>
@@ -685,23 +685,23 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="39.77734375" customWidth="1"/>
+    <col min="1" max="1" width="39.75" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="49.8">
+    <row r="1" spans="1:3" ht="50.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" ht="33.6" thickBot="1">
+    <row r="2" spans="1:3" ht="33" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -777,7 +777,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -804,7 +804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16.8" thickBot="1">
+    <row r="15" spans="1:3" ht="17.25" thickBot="1">
       <c r="A15" s="10" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
add function that stopping withdraw course when the total credits will under 9
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack9\Desktop\DB\DB_CourseSelectionSystem\Menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD8855B-D54F-4B17-9581-988D747E6C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1386E13C-7195-42D6-BA92-DFF1C543909D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
@@ -685,7 +685,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5"/>
@@ -769,7 +769,7 @@
         <v>7</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3">

</xml_diff>

<commit_message>
CHG: finish homeworktable when newuser give required course AND SQL required column change to 0,1
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack9\Desktop\DB\DB_CourseSelectionSystem\Menu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruserxd/Desktop/college/2down/DB_CourseSelectionSystem/Menu/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1386E13C-7195-42D6-BA92-DFF1C543909D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF57291A-78E7-464C-9988-AA2B380CCBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15840" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
   <sheets>
     <sheet name="功能表" sheetId="1" r:id="rId1"/>
@@ -685,23 +685,23 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="39.75" customWidth="1"/>
+    <col min="1" max="1" width="39.6640625" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="50.25">
+    <row r="1" spans="1:3" ht="50">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" ht="33" thickBot="1">
+    <row r="2" spans="1:3" ht="35" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -748,7 +748,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" ht="16">
       <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
@@ -785,7 +785,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -804,7 +804,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17.25" thickBot="1">
+    <row r="15" spans="1:3" ht="16" thickBot="1">
       <c r="A15" s="10" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
update to do list
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruserxd/Desktop/college/2down/DB_CourseSelectionSystem/Menu/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DB\Menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF57291A-78E7-464C-9988-AA2B380CCBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF650AA9-00B6-4ECA-9C21-18E085488161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15840" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
   <sheets>
     <sheet name="功能表" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="23">
   <si>
     <t>database_SelectedSystem</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -140,6 +138,30 @@
   </si>
   <si>
     <t>O</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>可選課列表：列出該同學可選的課程清單</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>關注抽籤功能</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>建立一個historyTable</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>評分(評分在history,在選課可以查看評分)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>搜索分類-&gt;你依照course的column列出相關課程</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>複製seletectedcourse就好了</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -311,7 +333,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -346,6 +368,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -682,26 +707,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD11E25E-09B4-E24C-BF54-4E794C068EA7}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="39.6640625" customWidth="1"/>
+    <col min="1" max="1" width="39.625" customWidth="1"/>
     <col min="2" max="2" width="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="50">
+    <row r="1" spans="1:3" ht="50.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:3" ht="35" thickBot="1">
+    <row r="2" spans="1:3" ht="33" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
@@ -748,7 +773,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="16">
+    <row r="8" spans="1:3">
       <c r="A8" s="9" t="s">
         <v>13</v>
       </c>
@@ -804,16 +829,45 @@
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="16" thickBot="1">
+    <row r="15" spans="1:3" ht="17.25" thickBot="1">
       <c r="A15" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="12" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
create history table and complete prerequisite course function
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\DB\Menu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jack9\Desktop\DB\Menu\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB22AB97-7D2D-4997-A9DE-AA4DA5ADA07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98602645-EEB2-4A53-BAF7-6323FC8AED3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="2475" windowWidth="24060" windowHeight="11295" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
+    <workbookView xWindow="6225" yWindow="2730" windowWidth="21600" windowHeight="11385" xr2:uid="{E2764C23-5740-1D4B-8AA3-216805C741EA}"/>
   </bookViews>
   <sheets>
     <sheet name="功能表" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="29">
   <si>
     <t>database_SelectedSystem</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,18 +161,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>複製seletectedcourse就好了</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>漢語</t>
   </si>
   <si>
     <t>漢語</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>X 林茂</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -364,7 +356,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -399,12 +391,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -743,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD11E25E-09B4-E24C-BF54-4E794C068EA7}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="150" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5" defaultRowHeight="16.5"/>
@@ -860,7 +846,7 @@
         <v>11</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="17.25" thickBot="1">
@@ -872,59 +858,59 @@
       </c>
     </row>
     <row r="16" spans="1:3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="8" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="7" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
+    <row r="19" spans="1:2">
+      <c r="A19" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="12" t="s">
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New teacher system can insert to SQL password:123
</commit_message>
<xml_diff>
--- a/Menu/makeSureWhatNeedToDo.xlsx
+++ b/Menu/makeSureWhatNeedToDo.xlsx
@@ -650,14 +650,14 @@
     <col min="3" max="3" style="13" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="48.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="48">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="34.5">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="35.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -709,7 +709,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="22.5">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="8" t="s">
         <v>9</v>
       </c>
@@ -790,7 +790,7 @@
       </c>
       <c r="C16" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="20.25">
       <c r="A17" s="6" t="s">
         <v>18</v>
       </c>
@@ -808,7 +808,7 @@
       </c>
       <c r="C18" s="5"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="21.75">
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="20.25">
       <c r="A19" s="6" t="s">
         <v>20</v>
       </c>

</xml_diff>